<commit_message>
[#10] chromedriver.exe exist in process when the task finished
</commit_message>
<xml_diff>
--- a/testcases/testcase1.xlsx
+++ b/testcases/testcase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0B3CAE-C7EA-4FC7-A211-135691D32CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2A6000-FDD2-448F-84CC-A87A30EF6A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>TestCase</t>
   </si>
@@ -80,14 +80,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>aaa</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>id=quick-search</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>run</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -143,6 +135,10 @@
   </si>
   <si>
     <t>cmd /C echo ${name}${password1}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${password1}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -526,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -545,13 +541,13 @@
     <col min="12" max="13" width="13.375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25" customWidth="1"/>
-    <col min="16" max="16" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36" customWidth="1"/>
-    <col min="18" max="18" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36" customWidth="1"/>
+    <col min="19" max="19" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.4">
@@ -559,16 +555,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -598,16 +594,16 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>5</v>
@@ -619,21 +615,21 @@
         <v>5</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -668,23 +664,23 @@
       <c r="P2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.4">
@@ -692,55 +688,55 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1</v>
+      <c r="R3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="S3" s="1">
         <v>1</v>
@@ -751,8 +747,8 @@
       <c r="U3" s="1">
         <v>1</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>19</v>
+      <c r="V3" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
@@ -785,19 +781,19 @@
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1">
-        <v>1</v>
-      </c>
+      <c r="R4" s="1"/>
       <c r="S4" s="1">
         <v>1</v>
       </c>
@@ -841,19 +837,19 @@
         <v>1</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O5" s="1"/>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1">
-        <v>1</v>
-      </c>
+      <c r="R5" s="1"/>
       <c r="S5" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
[#5] add read properties to stock variables and add save properties command
</commit_message>
<xml_diff>
--- a/testcases/testcase1.xlsx
+++ b/testcases/testcase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2A6000-FDD2-448F-84CC-A87A30EF6A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F52C60-DAD1-4F9A-8789-2CC2CE193EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>TestCase</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>${password1}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>saveProperties</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C:\Users\xihu_\Desktop\3.json</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name,password,age,password1</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -520,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -543,14 +555,14 @@
     <col min="15" max="15" width="25" customWidth="1"/>
     <col min="16" max="16" width="13.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36" customWidth="1"/>
-    <col min="19" max="19" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="36" customWidth="1"/>
+    <col min="20" max="20" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +618,7 @@
         <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>5</v>
@@ -617,8 +629,11 @@
       <c r="V1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="W1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -671,19 +686,22 @@
         <v>26</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -738,8 +756,8 @@
       <c r="R3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="1">
-        <v>1</v>
+      <c r="S3" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="T3" s="1">
         <v>1</v>
@@ -750,8 +768,11 @@
       <c r="V3" s="1">
         <v>1</v>
       </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -794,9 +815,7 @@
         <v>14</v>
       </c>
       <c r="R4" s="1"/>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
+      <c r="S4" s="1"/>
       <c r="T4" s="1">
         <v>1</v>
       </c>
@@ -806,8 +825,11 @@
       <c r="V4" s="1">
         <v>1</v>
       </c>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -850,9 +872,7 @@
         <v>14</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="1">
-        <v>1</v>
-      </c>
+      <c r="S5" s="1"/>
       <c r="T5" s="1">
         <v>1</v>
       </c>
@@ -860,6 +880,9 @@
         <v>1</v>
       </c>
       <c r="V5" s="1">
+        <v>1</v>
+      </c>
+      <c r="W5" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add increase number command
</commit_message>
<xml_diff>
--- a/testcases/testcase1.xlsx
+++ b/testcases/testcase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EAAC3C-E0DA-44E5-83A4-82465541D502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB92B8E-0575-43ED-B1D2-E5BDE2CD584C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>TestCase</t>
   </si>
@@ -158,7 +158,35 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{"name":"hugang","caseId":"hugangのテスト"}</t>
+    <t>https://build.hugang.io/job/test/job/buid</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jenkinsJob</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{ "userName": "${userName}", "token": "${token}", "parameters": { "BRANCH": "master", "APPS": "test1\ntest2" } }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{"userName":"hugang","caseId":"hugangのテスト"}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>age</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>increaseNumber</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1,3, </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>age,caseId</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -166,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -179,6 +207,14 @@
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -214,23 +250,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,38 +586,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:AA5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.875" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" customWidth="1"/>
-    <col min="5" max="6" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25" customWidth="1"/>
-    <col min="16" max="16" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="36" customWidth="1"/>
-    <col min="21" max="21" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.375" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="95.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.5" customWidth="1"/>
+    <col min="8" max="9" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25" customWidth="1"/>
+    <col min="19" max="19" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="36" customWidth="1"/>
+    <col min="24" max="24" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,25 +631,25 @@
         <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
@@ -612,43 +658,52 @@
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="Y1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -656,94 +711,103 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
       <c r="I3" s="1">
         <v>1</v>
       </c>
@@ -756,56 +820,61 @@
       <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="1">
-        <v>1</v>
-      </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U3" s="1">
-        <v>1</v>
-      </c>
-      <c r="V3" s="1">
-        <v>1</v>
-      </c>
-      <c r="W3" s="1">
-        <v>1</v>
-      </c>
       <c r="X3" s="1">
         <v>1</v>
       </c>
+      <c r="Y3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1">
         <v>1</v>
@@ -813,57 +882,60 @@
       <c r="I4" s="1">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
-        <v>1</v>
-      </c>
+      <c r="J4" s="1"/>
       <c r="K4" s="1">
         <v>1</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1"/>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1">
-        <v>1</v>
-      </c>
-      <c r="V4" s="1">
-        <v>1</v>
-      </c>
-      <c r="W4" s="1">
-        <v>1</v>
-      </c>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
       <c r="X4" s="1">
         <v>1</v>
       </c>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1">
         <v>1</v>
@@ -871,47 +943,57 @@
       <c r="I5" s="1">
         <v>1</v>
       </c>
-      <c r="J5" s="1">
-        <v>1</v>
-      </c>
+      <c r="J5" s="1"/>
       <c r="K5" s="1">
         <v>1</v>
       </c>
       <c r="L5" s="1">
         <v>1</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1"/>
+      <c r="S5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1">
-        <v>1</v>
-      </c>
-      <c r="V5" s="1">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1">
-        <v>1</v>
-      </c>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
       <c r="X5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{B2FBBD69-A743-4036-8324-11FF28CB72D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add mouse over command
</commit_message>
<xml_diff>
--- a/testcases/testcase1.xlsx
+++ b/testcases/testcase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBC831C-176C-4263-A99E-278FAF99EB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3FE4FA-7E6B-4004-B536-EC17B707B240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>TestCase</t>
   </si>
@@ -155,18 +155,6 @@
   </si>
   <si>
     <t>CaseNO_${caseId}_ログイン</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>https://build.hugang.io/job/test/job/buid</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>jenkinsJob</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{ "userName": "${userName}", "token": "${token}", "parameters": { "BRANCH": "master", "APPS": "test1\ntest2" } }</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -194,7 +182,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -207,14 +195,6 @@
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="游ゴシック"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -250,15 +230,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -268,12 +245,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -586,41 +559,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="47.25" customWidth="1"/>
     <col min="3" max="3" width="31.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.375" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
-    <col min="6" max="6" width="95.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.5" customWidth="1"/>
-    <col min="8" max="9" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25" customWidth="1"/>
-    <col min="19" max="19" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.75" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="36" customWidth="1"/>
-    <col min="24" max="24" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
+    <col min="7" max="8" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25" customWidth="1"/>
+    <col min="18" max="18" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.75" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="36" customWidth="1"/>
+    <col min="23" max="23" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,25 +603,25 @@
         <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>5</v>
@@ -664,31 +636,31 @@
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>5</v>
@@ -699,11 +671,8 @@
       <c r="Z1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -711,43 +680,43 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>39</v>
+      <c r="F2" t="s">
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
         <v>26</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>12</v>
@@ -758,56 +727,53 @@
       <c r="S2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="V2" t="s">
+      <c r="U2" t="s">
         <v>25</v>
       </c>
+      <c r="V2" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="W2" s="1" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
       <c r="I3" s="1">
         <v>1</v>
       </c>
@@ -826,33 +792,33 @@
       <c r="N3" s="1">
         <v>1</v>
       </c>
-      <c r="O3" s="1">
-        <v>1</v>
+      <c r="O3" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="T3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="1">
-        <v>1</v>
+      <c r="T3" s="1">
+        <v>1</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="W3" s="1">
+        <v>1</v>
+      </c>
       <c r="X3" s="1">
         <v>1</v>
       </c>
@@ -862,11 +828,8 @@
       <c r="Z3" s="1">
         <v>1</v>
       </c>
-      <c r="AA3" s="1">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -875,14 +838,16 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
       <c r="K4" s="1">
         <v>1</v>
       </c>
@@ -895,25 +860,25 @@
       <c r="N4" s="1">
         <v>1</v>
       </c>
-      <c r="O4" s="1">
-        <v>1</v>
+      <c r="O4" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
+      <c r="W4" s="1">
+        <v>1</v>
+      </c>
       <c r="X4" s="1">
         <v>1</v>
       </c>
@@ -923,11 +888,8 @@
       <c r="Z4" s="1">
         <v>1</v>
       </c>
-      <c r="AA4" s="1">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -936,14 +898,16 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
       <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1">
+        <v>1</v>
+      </c>
       <c r="K5" s="1">
         <v>1</v>
       </c>
@@ -956,25 +920,25 @@
       <c r="N5" s="1">
         <v>1</v>
       </c>
-      <c r="O5" s="1">
-        <v>1</v>
+      <c r="O5" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1" t="s">
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
+      <c r="W5" s="1">
+        <v>1</v>
+      </c>
       <c r="X5" s="1">
         <v>1</v>
       </c>
@@ -982,18 +946,12 @@
         <v>1</v>
       </c>
       <c r="Z5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{B2FBBD69-A743-4036-8324-11FF28CB72D9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor for if and times
</commit_message>
<xml_diff>
--- a/testcases/testcase1.xlsx
+++ b/testcases/testcase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F0C806-6957-4AD7-856A-891ABFD97E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871C6262-0F4F-46C7-B20C-0A73B9A5D2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>open</t>
   </si>
@@ -152,10 +152,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>{"userName":"hugang","caseId":"hugangのテスト"}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>age</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -184,10 +180,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>userName == 'hugang'</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>C:\Users\xihu_\Desktop\2.json</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -205,6 +197,18 @@
   </si>
   <si>
     <t>${userName}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{"userName":"hugang","caseId":"hugangのテスト","times":"5"}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>${times}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>userName == 'hugang' &amp;&amp; parseInt(times) == 5</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -632,16 +636,16 @@
   <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="4.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.375" bestFit="1" customWidth="1"/>
@@ -672,7 +676,7 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
@@ -681,25 +685,25 @@
         <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>32</v>
@@ -768,7 +772,7 @@
         <v>4</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.4">
@@ -779,19 +783,19 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" t="s">
         <v>45</v>
       </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>33</v>
@@ -866,10 +870,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -878,10 +882,10 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
refactor add run case command
</commit_message>
<xml_diff>
--- a/testcases/testcase1.xlsx
+++ b/testcases/testcase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projs\auto-test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871C6262-0F4F-46C7-B20C-0A73B9A5D2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BBB263C-D63D-4C78-9F40-BD22BB24F6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>open</t>
   </si>
@@ -209,6 +209,14 @@
   </si>
   <si>
     <t>userName == 'hugang' &amp;&amp; parseInt(times) == 5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>runCase</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlsx,C:\projs\auto-test\testcases\testcase2.xlsx</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -297,7 +305,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -311,9 +319,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
@@ -633,48 +638,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG5"/>
+  <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:AH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="34.875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.75" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.75" customWidth="1"/>
+    <col min="4" max="4" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="34.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.25" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -682,46 +688,46 @@
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>4</v>
@@ -736,102 +742,105 @@
         <v>4</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AF1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="O2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>11</v>
@@ -842,60 +851,63 @@
       <c r="Y2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AG2" s="6"/>
+      <c r="AH2" s="5"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="1">
-        <v>1</v>
-      </c>
       <c r="O3" s="1">
         <v>1</v>
       </c>
@@ -914,45 +926,48 @@
       <c r="T3" s="1">
         <v>1</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC3" s="1">
-        <v>1</v>
-      </c>
       <c r="AD3" s="1">
         <v>1</v>
       </c>
-      <c r="AE3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="6"/>
+      <c r="AE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="5"/>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -967,16 +982,14 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
+      <c r="M4" s="1"/>
       <c r="N4" s="1">
         <v>1</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1">
-        <v>1</v>
-      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1"/>
       <c r="Q4" s="1">
         <v>1</v>
       </c>
@@ -989,37 +1002,40 @@
       <c r="T4" s="1">
         <v>1</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="1" t="s">
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
-      <c r="AC4" s="1">
-        <v>1</v>
-      </c>
+      <c r="AC4" s="1"/>
       <c r="AD4" s="1">
         <v>1</v>
       </c>
-      <c r="AE4" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="6"/>
+      <c r="AE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="5"/>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1034,16 +1050,14 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
+      <c r="M5" s="1"/>
       <c r="N5" s="1">
         <v>1</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1">
-        <v>1</v>
-      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1">
         <v>1</v>
       </c>
@@ -1056,35 +1070,38 @@
       <c r="T5" s="1">
         <v>1</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="1">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="1" t="s">
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="1">
-        <v>1</v>
-      </c>
+      <c r="AC5" s="1"/>
       <c r="AD5" s="1">
         <v>1</v>
       </c>
-      <c r="AE5" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="6"/>
+      <c r="AE5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>